<commit_message>
Stability, organization, some cool new stuff
most notably, a new script to disable Windows' ALT menu acceleration, a
feature that i have LONG HATED
</commit_message>
<xml_diff>
--- a/FYI/Table_of_all_scan_codes.xlsx
+++ b/FYI/Table_of_all_scan_codes.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -73,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D195" authorId="0">
+    <comment ref="D205" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="588">
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Web/API/KeyboardEvent/code</t>
   </si>
@@ -815,9 +814,6 @@
     <t>6B</t>
   </si>
   <si>
-    <t>0D</t>
-  </si>
-  <si>
     <t>SC11C</t>
   </si>
   <si>
@@ -1010,9 +1006,6 @@
     <t>EB</t>
   </si>
   <si>
-    <t>{NumpadEnter}</t>
-  </si>
-  <si>
     <t>SC0E8</t>
   </si>
   <si>
@@ -1343,9 +1336,6 @@
     <t>free? - this WAS right CTRL</t>
   </si>
   <si>
-    <t>1d,0,1 is left… 1d,0,2 is right……</t>
-  </si>
-  <si>
     <t>keyboard Lang 3</t>
   </si>
   <si>
@@ -1625,9 +1615,6 @@
     <t>https://jacksautohotkeyblog.wordpress.com/2016/04/14/understanding-autohotkey-keyboard-scan-codes-and-virtual-key-codes-beginning-hotkeys-part-12/</t>
   </si>
   <si>
-    <t>Ignore all this, I don't remember where it came from</t>
-  </si>
-  <si>
     <t>Jelly comb numpad (not anymore)</t>
   </si>
   <si>
@@ -1652,9 +1639,6 @@
     <t>extra keyboard via Intercept.exe:  rightWin (AZIO keyboard)</t>
   </si>
   <si>
-    <t>extra keyboard via Intercept.exe: rightCtrl (Azio keyboard)</t>
-  </si>
-  <si>
     <t>Back</t>
   </si>
   <si>
@@ -1680,6 +1664,207 @@
   </si>
   <si>
     <t>In my experiments, I've had difficulty getting AHK to recognise scan codes 080 and higher…</t>
+  </si>
+  <si>
+    <t>SC110</t>
+  </si>
+  <si>
+    <t>SC119</t>
+  </si>
+  <si>
+    <t>SC124</t>
+  </si>
+  <si>
+    <t>SC122</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>SC06B ?</t>
+  </si>
+  <si>
+    <t>SC021 ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media_Prev </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media_Next    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media_Stop   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume_Mute    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume_Down    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume_Up   </t>
+  </si>
+  <si>
+    <t>//////</t>
+  </si>
+  <si>
+    <t>SC155</t>
+  </si>
+  <si>
+    <t>SC156</t>
+  </si>
+  <si>
+    <t>SC157</t>
+  </si>
+  <si>
+    <t>SC158</t>
+  </si>
+  <si>
+    <t>SC159</t>
+  </si>
+  <si>
+    <t>SC111</t>
+  </si>
+  <si>
+    <t>SC112</t>
+  </si>
+  <si>
+    <t>SC113</t>
+  </si>
+  <si>
+    <t>SC114</t>
+  </si>
+  <si>
+    <t>SC115</t>
+  </si>
+  <si>
+    <t>SC116</t>
+  </si>
+  <si>
+    <t>SC117</t>
+  </si>
+  <si>
+    <t>SC118</t>
+  </si>
+  <si>
+    <t>SC11A</t>
+  </si>
+  <si>
+    <t>SC11B</t>
+  </si>
+  <si>
+    <t>SC11E</t>
+  </si>
+  <si>
+    <t>SC11F</t>
+  </si>
+  <si>
+    <t>SC120</t>
+  </si>
+  <si>
+    <t>SC121</t>
+  </si>
+  <si>
+    <t>SC123</t>
+  </si>
+  <si>
+    <t>SC125</t>
+  </si>
+  <si>
+    <t>SC126</t>
+  </si>
+  <si>
+    <t>SC127</t>
+  </si>
+  <si>
+    <t>SC128</t>
+  </si>
+  <si>
+    <t>SC129</t>
+  </si>
+  <si>
+    <t>SC12A</t>
+  </si>
+  <si>
+    <t>SC12B</t>
+  </si>
+  <si>
+    <t>SC12C</t>
+  </si>
+  <si>
+    <t>SC12D</t>
+  </si>
+  <si>
+    <t>SC12E</t>
+  </si>
+  <si>
+    <t>SC12F</t>
+  </si>
+  <si>
+    <t>SC130</t>
+  </si>
+  <si>
+    <t>SC131</t>
+  </si>
+  <si>
+    <t>SC134</t>
+  </si>
+  <si>
+    <t>/////</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>??????</t>
+  </si>
+  <si>
+    <t>???? Not sure if this is right…</t>
+  </si>
+  <si>
+    <t>SC137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Down    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Up   </t>
+  </si>
+  <si>
+    <t>Previous Track</t>
+  </si>
+  <si>
+    <t>Next track</t>
+  </si>
+  <si>
+    <t>Mute</t>
+  </si>
+  <si>
+    <t>Play/Pause</t>
+  </si>
+  <si>
+    <t>Media Stop</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Right Ctrl</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Left Ctrl</t>
+  </si>
+  <si>
+    <t>TERRIBLE IDEA, MUST FIX: extra keyboard via Intercept.exe: rightCtrl (Azio keyboard)</t>
+  </si>
+  <si>
+    <t>in intercept.exe:  1d,0,1 is left -- 1d,0,2 is right</t>
+  </si>
+  <si>
+    <t>Ignore all this, I don't remember where it came from or if it is even accurate, they seem to be wrong by 100.</t>
   </si>
 </sst>
 </file>
@@ -1989,7 +2174,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2088,6 +2273,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -2391,11 +2577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O217"/>
+  <dimension ref="A1:O256"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G137" sqref="G137"/>
+      <pane ySplit="2" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2422,79 +2608,79 @@
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
       <c r="F1" s="39" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
       <c r="O1" s="41" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="43" customFormat="1" ht="15" thickBot="1">
       <c r="A2" s="42"/>
       <c r="B2" s="43" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>412</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="H2" s="46" t="s">
         <v>405</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>415</v>
-      </c>
-      <c r="G2" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>407</v>
       </c>
       <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:15" s="25" customFormat="1">
       <c r="B3" s="30" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H3" s="28"/>
       <c r="O3" s="29"/>
     </row>
     <row r="4" spans="1:15" s="25" customFormat="1">
       <c r="B4" s="31" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>436</v>
       </c>
-      <c r="E4" s="25" t="s">
-        <v>518</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>439</v>
-      </c>
       <c r="G4" s="27" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H4" s="28"/>
       <c r="O4" s="29"/>
@@ -2517,23 +2703,23 @@
         <v>128</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F7" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="20"/>
@@ -2541,16 +2727,16 @@
     <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F8" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="20"/>
@@ -2599,9 +2785,6 @@
       <c r="D13" s="6">
         <v>3</v>
       </c>
-      <c r="O13" s="11" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1"/>
@@ -2620,6 +2803,9 @@
       <c r="D15" s="6">
         <v>5</v>
       </c>
+      <c r="O15" s="11" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1"/>
@@ -2639,7 +2825,7 @@
         <v>7</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -2651,7 +2837,7 @@
         <v>8</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -2663,7 +2849,7 @@
         <v>9</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -2675,10 +2861,10 @@
         <v>178</v>
       </c>
       <c r="I20" t="s">
-        <v>507</v>
+        <v>587</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2690,10 +2876,10 @@
         <v>179</v>
       </c>
       <c r="I21" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2705,14 +2891,14 @@
         <v>130</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K22" s="48"/>
       <c r="O22" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2724,16 +2910,16 @@
         <v>131</v>
       </c>
       <c r="I23" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J23" s="48" t="s">
         <v>106</v>
       </c>
       <c r="K23" s="49" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2745,16 +2931,16 @@
         <v>181</v>
       </c>
       <c r="I24" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J24" s="48" t="s">
         <v>105</v>
       </c>
       <c r="K24" s="49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O24" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -2766,16 +2952,16 @@
         <v>180</v>
       </c>
       <c r="I25" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J25" s="48" t="s">
         <v>103</v>
       </c>
       <c r="K25" s="49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -2787,16 +2973,16 @@
         <v>182</v>
       </c>
       <c r="I26" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J26" s="48" t="s">
         <v>104</v>
       </c>
       <c r="K26" s="49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -2808,16 +2994,16 @@
         <v>183</v>
       </c>
       <c r="I27" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J27" s="48" t="s">
         <v>101</v>
       </c>
       <c r="K27" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O27" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -2829,16 +3015,16 @@
         <v>185</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J28" s="48" t="s">
         <v>102</v>
       </c>
       <c r="K28" s="49" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2850,16 +3036,16 @@
         <v>184</v>
       </c>
       <c r="I29" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J29" s="48" t="s">
         <v>51</v>
       </c>
       <c r="K29" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O29" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2871,16 +3057,16 @@
         <v>186</v>
       </c>
       <c r="I30" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J30" s="48" t="s">
         <v>33</v>
       </c>
       <c r="K30" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2892,16 +3078,16 @@
         <v>187</v>
       </c>
       <c r="I31" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J31" s="48" t="s">
         <v>47</v>
       </c>
       <c r="K31" s="49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2916,7 +3102,7 @@
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
       <c r="O32" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -2932,16 +3118,16 @@
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="I33" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J33" s="50" t="s">
         <v>26</v>
       </c>
       <c r="K33" s="51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O33" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2953,16 +3139,16 @@
         <v>190</v>
       </c>
       <c r="I34" s="48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J34" s="48" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O34" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -2974,16 +3160,16 @@
         <v>191</v>
       </c>
       <c r="I35" s="48" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J35" s="48" t="s">
         <v>37</v>
       </c>
       <c r="K35" s="49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O35" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2994,36 +3180,46 @@
       <c r="D36" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="48" t="s">
+        <v>525</v>
+      </c>
+      <c r="J36" s="48" t="s">
+        <v>35</v>
+      </c>
       <c r="K36" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O36" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="1"/>
+      <c r="B37" s="3" t="s">
+        <v>583</v>
+      </c>
       <c r="C37" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E37" t="s">
-        <v>413</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>516</v>
+        <v>586</v>
+      </c>
+      <c r="F37" t="s">
+        <v>584</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="I37" s="48"/>
       <c r="J37" s="48"/>
       <c r="K37" s="49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O37" s="11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -3037,10 +3233,10 @@
       <c r="I38" s="48"/>
       <c r="J38" s="48"/>
       <c r="K38" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O38" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -3055,7 +3251,7 @@
       <c r="J39" s="48"/>
       <c r="K39" s="48"/>
       <c r="O39" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -3067,16 +3263,16 @@
         <v>216</v>
       </c>
       <c r="I40" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J40" s="48" t="s">
-        <v>107</v>
+        <v>526</v>
       </c>
       <c r="K40" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -3091,16 +3287,16 @@
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="I41" s="50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J41" s="50" t="s">
-        <v>34</v>
+        <v>527</v>
       </c>
       <c r="K41" s="51" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O41" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -3115,7 +3311,7 @@
       <c r="J42" s="48"/>
       <c r="K42" s="48"/>
       <c r="O42" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -3130,7 +3326,7 @@
       <c r="J43" s="48"/>
       <c r="K43" s="48"/>
       <c r="O43" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -3145,7 +3341,7 @@
       <c r="J44" s="48"/>
       <c r="K44" s="48"/>
       <c r="O44" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -3160,7 +3356,7 @@
       <c r="J45" s="48"/>
       <c r="K45" s="48"/>
       <c r="O45" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -3175,7 +3371,7 @@
       <c r="J46" s="48"/>
       <c r="K46" s="48"/>
       <c r="O46" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -3190,7 +3386,7 @@
       <c r="J47" s="48"/>
       <c r="K47" s="48"/>
       <c r="O47" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -3205,7 +3401,7 @@
       <c r="J48" s="48"/>
       <c r="K48" s="48"/>
       <c r="O48" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -3220,7 +3416,7 @@
       <c r="J49" s="48"/>
       <c r="K49" s="48"/>
       <c r="O49" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -3235,13 +3431,13 @@
       <c r="J50" s="48"/>
       <c r="K50" s="48"/>
       <c r="O50" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="1"/>
       <c r="B51" s="3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>44</v>
@@ -3250,13 +3446,13 @@
         <v>197</v>
       </c>
       <c r="F51" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I51" s="48"/>
       <c r="J51" s="48"/>
       <c r="K51" s="48"/>
       <c r="O51" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -3271,7 +3467,7 @@
       <c r="J52" s="48"/>
       <c r="K52" s="48"/>
       <c r="O52" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -3286,7 +3482,7 @@
       <c r="J53" s="48"/>
       <c r="K53" s="48"/>
       <c r="O53" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="54" spans="1:15">
@@ -3301,7 +3497,7 @@
       <c r="J54" s="48"/>
       <c r="K54" s="48"/>
       <c r="O54" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -3316,7 +3512,7 @@
       <c r="J55" s="48"/>
       <c r="K55" s="48"/>
       <c r="O55" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="56" spans="1:15">
@@ -3328,16 +3524,16 @@
         <v>201</v>
       </c>
       <c r="I56" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J56" s="48" t="s">
         <v>49</v>
       </c>
       <c r="K56" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O56" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="57" spans="1:15">
@@ -3349,7 +3545,7 @@
         <v>202</v>
       </c>
       <c r="O57" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -3361,7 +3557,7 @@
         <v>203</v>
       </c>
       <c r="O58" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -3373,7 +3569,7 @@
         <v>204</v>
       </c>
       <c r="O59" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="60" spans="1:15">
@@ -3385,7 +3581,7 @@
         <v>205</v>
       </c>
       <c r="O60" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="61" spans="1:15">
@@ -3397,7 +3593,7 @@
         <v>206</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="62" spans="1:15">
@@ -3409,7 +3605,7 @@
         <v>195</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="63" spans="1:15">
@@ -3421,7 +3617,7 @@
         <v>234</v>
       </c>
       <c r="O63" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -3433,7 +3629,7 @@
         <v>220</v>
       </c>
       <c r="O64" s="11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="65" spans="1:15">
@@ -3445,7 +3641,7 @@
         <v>221</v>
       </c>
       <c r="O65" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66" spans="1:15">
@@ -3457,7 +3653,7 @@
         <v>222</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67" spans="1:15">
@@ -3469,7 +3665,7 @@
         <v>133</v>
       </c>
       <c r="O67" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="68" spans="1:15">
@@ -3481,7 +3677,7 @@
         <v>134</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="69" spans="1:15">
@@ -3493,7 +3689,7 @@
         <v>135</v>
       </c>
       <c r="O69" s="11" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70" spans="1:15">
@@ -3505,7 +3701,7 @@
         <v>136</v>
       </c>
       <c r="O70" s="11" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:15">
@@ -3517,7 +3713,7 @@
         <v>137</v>
       </c>
       <c r="O71" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="72" spans="1:15">
@@ -3529,7 +3725,7 @@
         <v>138</v>
       </c>
       <c r="O72" s="11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73" spans="1:15">
@@ -3541,7 +3737,7 @@
         <v>139</v>
       </c>
       <c r="O73" s="11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="74" spans="1:15">
@@ -3553,7 +3749,7 @@
         <v>140</v>
       </c>
       <c r="O74" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -3565,7 +3761,7 @@
         <v>141</v>
       </c>
       <c r="O75" s="11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="76" spans="1:15">
@@ -3577,7 +3773,7 @@
         <v>142</v>
       </c>
       <c r="O76" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="77" spans="1:15">
@@ -3592,7 +3788,7 @@
         <v>223</v>
       </c>
       <c r="O77" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="78" spans="1:15">
@@ -3604,7 +3800,7 @@
         <v>144</v>
       </c>
       <c r="O78" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="79" spans="1:15">
@@ -3619,7 +3815,7 @@
         <v>145</v>
       </c>
       <c r="O79" s="11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="80" spans="1:15">
@@ -3634,7 +3830,7 @@
         <v>146</v>
       </c>
       <c r="O80" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="81" spans="1:15">
@@ -3649,13 +3845,13 @@
         <v>147</v>
       </c>
       <c r="O81" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="82" spans="1:15">
       <c r="A82" s="1"/>
       <c r="B82" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>75</v>
@@ -3664,7 +3860,7 @@
         <v>235</v>
       </c>
       <c r="O82" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="83" spans="1:15">
@@ -3679,7 +3875,7 @@
         <v>148</v>
       </c>
       <c r="O83" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="84" spans="1:15">
@@ -3694,7 +3890,7 @@
         <v>149</v>
       </c>
       <c r="O84" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="85" spans="1:15">
@@ -3709,7 +3905,7 @@
         <v>150</v>
       </c>
       <c r="O85" s="11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="86" spans="1:15">
@@ -3724,7 +3920,7 @@
         <v>151</v>
       </c>
       <c r="O86" s="11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="87" spans="1:15">
@@ -3739,7 +3935,7 @@
         <v>152</v>
       </c>
       <c r="O87" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="88" spans="1:15">
@@ -3754,7 +3950,7 @@
         <v>153</v>
       </c>
       <c r="O88" s="11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="89" spans="1:15">
@@ -3769,7 +3965,7 @@
         <v>154</v>
       </c>
       <c r="O89" s="11" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="90" spans="1:15">
@@ -3784,31 +3980,31 @@
         <v>155</v>
       </c>
       <c r="O90" s="11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="91" spans="1:15">
       <c r="A91" s="1"/>
       <c r="B91" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E91" s="24" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="O91" s="11" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="92" spans="1:15">
       <c r="A92" s="1"/>
       <c r="B92" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>127</v>
@@ -3817,7 +4013,7 @@
         <v>156</v>
       </c>
       <c r="O92" s="11" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="93" spans="1:15">
@@ -3829,13 +4025,13 @@
         <v>128</v>
       </c>
       <c r="O93" s="11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="94" spans="1:15">
       <c r="A94" s="1"/>
       <c r="B94" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>86</v>
@@ -3844,19 +4040,19 @@
         <v>197</v>
       </c>
       <c r="E94" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F94" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="O94" s="11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="95" spans="1:15">
       <c r="A95" s="1"/>
       <c r="B95" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>87</v>
@@ -3865,13 +4061,13 @@
         <v>157</v>
       </c>
       <c r="O95" s="11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="96" spans="1:15">
       <c r="A96" s="1"/>
       <c r="B96" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>88</v>
@@ -3880,31 +4076,31 @@
         <v>158</v>
       </c>
       <c r="O96" s="11" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="97" spans="1:15">
       <c r="A97" s="1"/>
       <c r="B97" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E97" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O97" s="11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" s="1"/>
       <c r="B98" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>90</v>
@@ -3913,10 +4109,10 @@
         <v>128</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="O98" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="99" spans="1:15">
@@ -3931,13 +4127,13 @@
         <v>128</v>
       </c>
       <c r="O99" s="11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" s="1"/>
       <c r="B100" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>92</v>
@@ -3946,13 +4142,13 @@
         <v>128</v>
       </c>
       <c r="F100" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G100" s="15" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="O100" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="101" spans="1:15">
@@ -3964,7 +4160,7 @@
         <v>128</v>
       </c>
       <c r="O101" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="102" spans="1:15">
@@ -3976,7 +4172,7 @@
         <v>128</v>
       </c>
       <c r="O102" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="103" spans="1:15" ht="13.5" customHeight="1">
@@ -3988,7 +4184,7 @@
         <v>128</v>
       </c>
       <c r="O103" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" spans="1:15">
@@ -4000,10 +4196,10 @@
         <v>128</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="O104" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="105" spans="1:15">
@@ -4015,16 +4211,16 @@
         <v>128</v>
       </c>
       <c r="G105" s="15" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="O105" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="106" spans="1:15">
       <c r="A106" s="1"/>
       <c r="B106" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>98</v>
@@ -4033,28 +4229,28 @@
         <v>128</v>
       </c>
       <c r="G106" s="21" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="O106" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="107" spans="1:15">
       <c r="A107" s="1"/>
       <c r="B107" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G107" s="15" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="O107" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="108" spans="1:15">
@@ -4066,10 +4262,10 @@
         <v>159</v>
       </c>
       <c r="G108" s="15" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="O108" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="109" spans="1:15">
@@ -4081,10 +4277,10 @@
         <v>160</v>
       </c>
       <c r="G109" s="15" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="O109" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="110" spans="1:15">
@@ -4096,10 +4292,10 @@
         <v>161</v>
       </c>
       <c r="G110" s="15" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O110" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="111" spans="1:15">
@@ -4111,10 +4307,10 @@
         <v>162</v>
       </c>
       <c r="G111" s="21" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="O111" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="112" spans="1:15">
@@ -4126,10 +4322,10 @@
         <v>163</v>
       </c>
       <c r="G112" s="15" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="O112" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="113" spans="1:15">
@@ -4141,10 +4337,10 @@
         <v>164</v>
       </c>
       <c r="G113" s="15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="O113" s="11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="114" spans="1:15">
@@ -4156,10 +4352,10 @@
         <v>165</v>
       </c>
       <c r="G114" s="15" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="O114" s="11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="115" spans="1:15">
@@ -4171,10 +4367,10 @@
         <v>166</v>
       </c>
       <c r="G115" s="15" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="O115" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="116" spans="1:15">
@@ -4195,7 +4391,7 @@
         <v>168</v>
       </c>
       <c r="G117" s="52" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="118" spans="1:15">
@@ -4207,7 +4403,7 @@
         <v>169</v>
       </c>
       <c r="G118" s="53" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="119" spans="1:15">
@@ -4219,7 +4415,7 @@
         <v>128</v>
       </c>
       <c r="G119" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="120" spans="1:15">
@@ -4237,7 +4433,7 @@
         <v>170</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G120" s="16"/>
       <c r="H120" s="18"/>
@@ -4245,7 +4441,7 @@
     <row r="121" spans="1:15">
       <c r="A121" s="1"/>
       <c r="B121" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>113</v>
@@ -4257,10 +4453,10 @@
         <v>171</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G121" s="23" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H121" s="18"/>
     </row>
@@ -4276,17 +4472,17 @@
         <v>172</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G122" s="23" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H122" s="18"/>
     </row>
     <row r="123" spans="1:15">
       <c r="A123" s="1"/>
       <c r="B123" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>115</v>
@@ -4298,7 +4494,7 @@
         <v>173</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G123" s="16"/>
       <c r="H123" s="18"/>
@@ -4312,7 +4508,7 @@
         <v>128</v>
       </c>
       <c r="G124" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:15">
@@ -4324,7 +4520,7 @@
         <v>128</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="126" spans="1:15">
@@ -4333,16 +4529,16 @@
         <v>87</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D126" s="10" t="s">
         <v>174</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G126" s="53" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="127" spans="1:15">
@@ -4354,10 +4550,10 @@
         <v>128</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="128" spans="1:15">
@@ -4369,16 +4565,16 @@
         <v>128</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="1"/>
       <c r="B129" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>120</v>
@@ -4390,11 +4586,11 @@
         <v>175</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G129" s="16"/>
       <c r="H129" s="18" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -4406,13 +4602,13 @@
         <v>128</v>
       </c>
       <c r="G130" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="131" spans="1:8">
       <c r="A131" s="1"/>
       <c r="B131" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>122</v>
@@ -4424,10 +4620,10 @@
         <v>176</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G131" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H131" s="18"/>
     </row>
@@ -4440,13 +4636,13 @@
         <v>128</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" s="1"/>
       <c r="B133" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>124</v>
@@ -4458,7 +4654,7 @@
         <v>177</v>
       </c>
       <c r="F133" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G133" s="16"/>
       <c r="H133" s="18"/>
@@ -4466,7 +4662,7 @@
     <row r="134" spans="1:8">
       <c r="A134" s="1"/>
       <c r="B134" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>125</v>
@@ -4475,7 +4671,7 @@
         <v>128</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -4490,399 +4686,685 @@
         <v>128</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="136" spans="1:8">
       <c r="C136" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G136" s="21" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="137" spans="1:8">
       <c r="C137" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="138" spans="1:8">
       <c r="C138" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="139" spans="1:8">
       <c r="C139" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="140" spans="1:8">
       <c r="C140" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="141" spans="1:8">
       <c r="C141" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="142" spans="1:8">
       <c r="C142" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="143" spans="1:8">
       <c r="C143" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="144" spans="1:8">
       <c r="C144" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="145" spans="3:3">
       <c r="C145" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="146" spans="3:3">
       <c r="C146" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="147" spans="3:3">
       <c r="C147" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="148" spans="3:3">
       <c r="C148" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="149" spans="3:3">
       <c r="C149" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="150" spans="3:3">
       <c r="C150" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="151" spans="3:3">
       <c r="C151" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="153" spans="3:3">
       <c r="C153" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="154" spans="3:3">
       <c r="C154" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="155" spans="3:3">
       <c r="C155" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="156" spans="3:3">
       <c r="C156" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="157" spans="3:3">
       <c r="C157" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="158" spans="3:3">
       <c r="C158" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="159" spans="3:3">
       <c r="C159" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="160" spans="3:3">
       <c r="C160" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="161" spans="3:4">
       <c r="C161" s="2" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="162" spans="3:4">
       <c r="C162" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="164" spans="3:4">
       <c r="C164" s="2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="165" spans="3:4">
       <c r="C165" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="166" spans="3:4">
       <c r="C166" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="167" spans="3:4">
       <c r="C167" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="170" spans="3:4">
       <c r="C170" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="173" spans="3:4">
       <c r="C173" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="174" spans="3:4">
       <c r="C174" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="175" spans="3:4">
       <c r="C175" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="176" spans="3:4">
       <c r="C176" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="177" spans="2:6">
+      <c r="C177" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="178" spans="2:6">
+      <c r="C178" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="179" spans="2:6">
+      <c r="C179" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="180" spans="2:6">
+      <c r="C180" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="181" spans="2:6">
+      <c r="C181" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="182" spans="2:6">
+      <c r="C182" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="177" spans="3:4">
-      <c r="C177" s="2" t="s">
+    <row r="183" spans="2:6">
+      <c r="C183" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="178" spans="3:4">
-      <c r="C178" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="179" spans="3:4">
-      <c r="C179" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="180" spans="3:4">
-      <c r="C180" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="181" spans="3:4">
-      <c r="C181" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D181" s="5" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="182" spans="3:4">
-      <c r="C182" s="2" t="s">
+    <row r="184" spans="2:6">
+      <c r="C184" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6">
+      <c r="C185" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="183" spans="3:4">
-      <c r="C183" s="2" t="s">
+    <row r="186" spans="2:6">
+      <c r="C186" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="184" spans="3:4">
-      <c r="C184" s="2" t="s">
+    <row r="187" spans="2:6">
+      <c r="C187" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="185" spans="3:4">
-      <c r="C185" s="2" t="s">
+    <row r="188" spans="2:6">
+      <c r="C188" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="186" spans="3:4">
-      <c r="C186" s="2" t="s">
+    <row r="190" spans="2:6">
+      <c r="C190" s="2" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="187" spans="3:4">
-      <c r="C187" s="2" t="s">
+      <c r="D190" s="5" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="188" spans="3:4">
-      <c r="C188" s="2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="191" spans="3:4">
-      <c r="C191" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="D191" s="5" t="s">
-        <v>502</v>
+    <row r="192" spans="2:6">
+      <c r="B192" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D192" t="s">
+        <v>528</v>
+      </c>
+      <c r="F192" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7">
+      <c r="C193" s="54" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="194" spans="2:7">
-      <c r="B194" s="3" t="s">
+      <c r="C194" s="54" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7">
+      <c r="C195" s="54" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7">
+      <c r="C196" s="54" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7">
+      <c r="C197" s="54" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7">
+      <c r="C198" s="54" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7">
+      <c r="C199" s="54" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7">
+      <c r="C200" s="54" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7">
+      <c r="B201" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="D201" t="s">
+        <v>529</v>
+      </c>
+      <c r="F201" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7">
+      <c r="C202" s="54" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7">
+      <c r="C203" s="54" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7">
+      <c r="C204" s="54" t="s">
         <v>237</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D194" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="195" spans="2:7">
-      <c r="C195" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D195" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="G195" s="15" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="197" spans="2:7">
-      <c r="C197" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D197" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="198" spans="2:7">
-      <c r="C198" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D198" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="201" spans="2:7">
-      <c r="C201" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D201" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="202" spans="2:7">
-      <c r="B202" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="203" spans="2:7">
-      <c r="B203" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D203" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="204" spans="2:7">
-      <c r="B204" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D204" s="5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="205" spans="2:7">
       <c r="B205" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D205" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="F205" t="s">
+        <v>582</v>
+      </c>
+      <c r="G205" s="15" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7">
+      <c r="C206" s="54" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7">
+      <c r="C207" s="54" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7">
+      <c r="B208" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="D208" t="s">
+        <v>531</v>
+      </c>
+      <c r="F208" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6">
+      <c r="C209" s="54" t="s">
+        <v>553</v>
+      </c>
+      <c r="D209"/>
+    </row>
+    <row r="210" spans="2:6">
+      <c r="B210" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="D210" t="s">
+        <v>269</v>
+      </c>
+      <c r="F210" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6">
+      <c r="C211" s="54" t="s">
+        <v>554</v>
+      </c>
+      <c r="D211"/>
+    </row>
+    <row r="212" spans="2:6">
+      <c r="B212" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D212" t="s">
+        <v>530</v>
+      </c>
+      <c r="F212" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="213" spans="2:6">
+      <c r="C213" s="54" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="214" spans="2:6">
+      <c r="C214" s="54" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="215" spans="2:6">
+      <c r="C215" s="54" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="216" spans="2:6">
+      <c r="C216" s="54" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="217" spans="2:6">
+      <c r="C217" s="54" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="218" spans="2:6">
+      <c r="C218" s="54" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="219" spans="2:6">
+      <c r="C219" s="54" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="220" spans="2:6">
+      <c r="C220" s="54" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="221" spans="2:6">
+      <c r="C221" s="54" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="222" spans="2:6">
+      <c r="B222" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D222" t="s">
+        <v>532</v>
+      </c>
+      <c r="F222" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="223" spans="2:6">
+      <c r="C223" s="54" t="s">
+        <v>565</v>
+      </c>
+      <c r="D223"/>
+    </row>
+    <row r="224" spans="2:6">
+      <c r="B224" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D224" t="s">
+        <v>533</v>
+      </c>
+      <c r="F224" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="225" spans="2:8">
+      <c r="C225" s="54" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="226" spans="2:8">
+      <c r="B226" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D226" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="227" spans="2:8">
+      <c r="C227" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D227" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="228" spans="2:8">
+      <c r="C228" s="54" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="229" spans="2:8">
+      <c r="C229" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D229" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="G229" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="H229" s="17" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="230" spans="2:8">
+      <c r="C230" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D230" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G230" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="H230" s="17" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="231" spans="2:8">
+      <c r="C231" s="54" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="233" spans="2:8">
+      <c r="C233" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="235" spans="2:8">
+      <c r="C235" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="236" spans="2:8">
+      <c r="C236" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="237" spans="2:8">
+      <c r="C237" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="238" spans="2:8">
+      <c r="C238" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="239" spans="2:8">
+      <c r="C239" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="240" spans="2:8">
+      <c r="C240" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4">
+      <c r="B241" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4">
+      <c r="B242" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4">
+      <c r="B243" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D243" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4">
+      <c r="B244" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D244" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4">
+      <c r="C247" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4">
+      <c r="C248"/>
+    </row>
+    <row r="250" spans="2:4">
+      <c r="B250" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C205" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D205" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4">
-      <c r="C209"/>
-    </row>
-    <row r="211" spans="2:4">
-      <c r="B211" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C211" s="2" t="s">
+      <c r="C250" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D250" s="5" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" ht="27">
+      <c r="C256" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="D211" s="5" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="214" spans="2:4">
-      <c r="B214" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D214" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="215" spans="2:4">
-      <c r="C215" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D215" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="217" spans="2:4" ht="27">
-      <c r="C217" s="4" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C217" r:id="rId1"/>
+    <hyperlink ref="C256" r:id="rId1"/>
     <hyperlink ref="O1" r:id="rId2"/>
     <hyperlink ref="A1" r:id="rId3"/>
     <hyperlink ref="F1" r:id="rId4"/>

</xml_diff>